<commit_message>
Building Main program for sezon table prediction
</commit_message>
<xml_diff>
--- a/Sezon/PremierLeague2025_26.xlsx
+++ b/Sezon/PremierLeague2025_26.xlsx
@@ -539,22 +539,22 @@
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5105004117165961</v>
+        <v>0.5057370115787179</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1989835724729284</v>
+        <v>0.2009199139923911</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2905160158104755</v>
+        <v>0.293343074428891</v>
       </c>
       <c r="L2" t="n">
-        <v>1.822017250960264</v>
+        <v>1.810554109165045</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8874667332292607</v>
+        <v>0.8961028164060643</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
@@ -667,25 +667,25 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="H5" t="n">
         <v>100</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3118558159110756</v>
+        <v>0.3177198620330348</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2797334081662294</v>
+        <v>0.2773496495800672</v>
       </c>
       <c r="K5" t="n">
-        <v>0.408410775922695</v>
+        <v>0.404930488386898</v>
       </c>
       <c r="L5" t="n">
-        <v>1.343978223655922</v>
+        <v>1.358090074486002</v>
       </c>
       <c r="M5" t="n">
-        <v>1.247611000421383</v>
+        <v>1.2369794371271</v>
       </c>
       <c r="N5" t="n">
         <v>3</v>
@@ -1149,25 +1149,25 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="H17" t="n">
         <v>100</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2196927826026768</v>
+        <v>0.2150822957514095</v>
       </c>
       <c r="J17" t="n">
-        <v>0.4595557547974151</v>
+        <v>0.4708975524515327</v>
       </c>
       <c r="K17" t="n">
-        <v>0.3207514625999081</v>
+        <v>0.3140201517970578</v>
       </c>
       <c r="L17" t="n">
-        <v>0.9798298104079386</v>
+        <v>0.9592670390512863</v>
       </c>
       <c r="M17" t="n">
-        <v>1.699418726992153</v>
+        <v>1.726712809151656</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1475,25 +1475,25 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="H25" t="n">
         <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2659489287035226</v>
+        <v>0.2529951550772887</v>
       </c>
       <c r="J25" t="n">
-        <v>0.3457656353893344</v>
+        <v>0.3776319185098698</v>
       </c>
       <c r="K25" t="n">
-        <v>0.388285435907143</v>
+        <v>0.3693729264128415</v>
       </c>
       <c r="L25" t="n">
-        <v>1.186132222017711</v>
+        <v>1.128358391644708</v>
       </c>
       <c r="M25" t="n">
-        <v>1.425582342075146</v>
+        <v>1.502268681942451</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -1567,25 +1567,25 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="H27" t="n">
         <v>100</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1796453014426486</v>
+        <v>0.1800361078507716</v>
       </c>
       <c r="J27" t="n">
-        <v>0.5580725584510846</v>
+        <v>0.5571111746871017</v>
       </c>
       <c r="K27" t="n">
-        <v>0.2622821401062669</v>
+        <v>0.2628527174621266</v>
       </c>
       <c r="L27" t="n">
-        <v>0.8012180444342125</v>
+        <v>0.8029610410144417</v>
       </c>
       <c r="M27" t="n">
-        <v>1.936499815459521</v>
+        <v>1.934186241523432</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -1623,22 +1623,22 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="I28" t="n">
-        <v>0.8479553947493842</v>
+        <v>0.856618248435607</v>
       </c>
       <c r="J28" t="n">
-        <v>0.06180675010187635</v>
+        <v>0.05828526486357438</v>
       </c>
       <c r="K28" t="n">
-        <v>0.09023785514873947</v>
+        <v>0.0850964867008186</v>
       </c>
       <c r="L28" t="n">
-        <v>2.634104039396892</v>
+        <v>2.654951232007639</v>
       </c>
       <c r="M28" t="n">
-        <v>0.2756581054543685</v>
+        <v>0.2599522812915417</v>
       </c>
       <c r="N28" t="n">
         <v>3</v>
@@ -1871,22 +1871,22 @@
         <v>100</v>
       </c>
       <c r="H34" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="I34" t="n">
-        <v>0.8143350188654325</v>
+        <v>0.822998722789835</v>
       </c>
       <c r="J34" t="n">
-        <v>0.07547356956689737</v>
+        <v>0.0719517387033191</v>
       </c>
       <c r="K34" t="n">
-        <v>0.1101914115676701</v>
+        <v>0.1050495385068459</v>
       </c>
       <c r="L34" t="n">
-        <v>2.553196468163967</v>
+        <v>2.574045706876351</v>
       </c>
       <c r="M34" t="n">
-        <v>0.3366121202683622</v>
+        <v>0.3209047546168032</v>
       </c>
       <c r="N34" t="n">
         <v>3</v>
@@ -1963,22 +1963,22 @@
         <v>100</v>
       </c>
       <c r="H36" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="I36" t="n">
-        <v>0.8491142560017515</v>
+        <v>0.8398570301250703</v>
       </c>
       <c r="J36" t="n">
-        <v>0.06133566829197095</v>
+        <v>0.06509876824184138</v>
       </c>
       <c r="K36" t="n">
-        <v>0.08955007570627758</v>
+        <v>0.09504420163308841</v>
       </c>
       <c r="L36" t="n">
-        <v>2.636892843711532</v>
+        <v>2.614615292008299</v>
       </c>
       <c r="M36" t="n">
-        <v>0.2735570805821904</v>
+        <v>0.2903405063586125</v>
       </c>
       <c r="N36" t="n">
         <v>3</v>
@@ -2364,25 +2364,25 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="H46" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="I46" t="n">
-        <v>0.6093942026776775</v>
+        <v>0.6321426031721259</v>
       </c>
       <c r="J46" t="n">
-        <v>0.1587828444399685</v>
+        <v>0.1495355271658025</v>
       </c>
       <c r="K46" t="n">
-        <v>0.231822952882354</v>
+        <v>0.2183218696620717</v>
       </c>
       <c r="L46" t="n">
-        <v>2.060005560915386</v>
+        <v>2.114749679178449</v>
       </c>
       <c r="M46" t="n">
-        <v>0.7081714862022594</v>
+        <v>0.6669284511594793</v>
       </c>
       <c r="N46" t="n">
         <v>0</v>
@@ -2612,25 +2612,25 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="H52" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="I52" t="n">
-        <v>0.6329264335192558</v>
+        <v>0.6475869796696524</v>
       </c>
       <c r="J52" t="n">
-        <v>0.1492168969433919</v>
+        <v>0.1432573253375397</v>
       </c>
       <c r="K52" t="n">
-        <v>0.2178566695373522</v>
+        <v>0.209155694992808</v>
       </c>
       <c r="L52" t="n">
-        <v>2.116635970095119</v>
+        <v>2.151916634001765</v>
       </c>
       <c r="M52" t="n">
-        <v>0.6655073603675281</v>
+        <v>0.638927671005427</v>
       </c>
       <c r="N52" t="n">
         <v>3</v>
@@ -2743,25 +2743,25 @@
         </is>
       </c>
       <c r="G55" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="H55" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="I55" t="n">
-        <v>0.2694342215318971</v>
+        <v>0.2664598175528735</v>
       </c>
       <c r="J55" t="n">
-        <v>0.337191815031533</v>
+        <v>0.3445088488199312</v>
       </c>
       <c r="K55" t="n">
-        <v>0.3933739634365698</v>
+        <v>0.3890313336271953</v>
       </c>
       <c r="L55" t="n">
-        <v>1.201676628032261</v>
+        <v>1.188410786285816</v>
       </c>
       <c r="M55" t="n">
-        <v>1.404949408531169</v>
+        <v>1.422557880086989</v>
       </c>
       <c r="N55" t="n">
         <v>3</v>
@@ -2874,25 +2874,25 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="H58" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="I58" t="n">
-        <v>0.702782380649092</v>
+        <v>0.7146787491073958</v>
       </c>
       <c r="J58" t="n">
-        <v>0.1208201704678488</v>
+        <v>0.115984248330327</v>
       </c>
       <c r="K58" t="n">
-        <v>0.1763974488830592</v>
+        <v>0.1693370025622774</v>
       </c>
       <c r="L58" t="n">
-        <v>2.284744590830336</v>
+        <v>2.313373249884465</v>
       </c>
       <c r="M58" t="n">
-        <v>0.5388579602866056</v>
+        <v>0.5172897475532583</v>
       </c>
       <c r="N58" t="n">
         <v>3</v>
@@ -3239,25 +3239,25 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="H67" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="I67" t="n">
-        <v>0.2551896203281747</v>
+        <v>0.2444711083301312</v>
       </c>
       <c r="J67" t="n">
-        <v>0.37223353399269</v>
+        <v>0.3986010735078772</v>
       </c>
       <c r="K67" t="n">
-        <v>0.3725768456791352</v>
+        <v>0.3569278181619916</v>
       </c>
       <c r="L67" t="n">
-        <v>1.138145706663659</v>
+        <v>1.090341143152385</v>
       </c>
       <c r="M67" t="n">
-        <v>1.489277447657205</v>
+        <v>1.552731038685623</v>
       </c>
       <c r="N67" t="n">
         <v>0</v>
@@ -3292,25 +3292,25 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="H68" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="I68" t="n">
-        <v>0.7916374569244052</v>
+        <v>0.8049532471849074</v>
       </c>
       <c r="J68" t="n">
-        <v>0.08470022076243691</v>
+        <v>0.07928729789231408</v>
       </c>
       <c r="K68" t="n">
-        <v>0.1236623223131579</v>
+        <v>0.1157594549227785</v>
       </c>
       <c r="L68" t="n">
-        <v>2.498574693086374</v>
+        <v>2.530619196477501</v>
       </c>
       <c r="M68" t="n">
-        <v>0.3777629846004686</v>
+        <v>0.3536213485997208</v>
       </c>
       <c r="N68" t="n">
         <v>3</v>
@@ -3579,25 +3579,25 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="H75" t="n">
-        <v>97.4048157878</v>
+        <v>97.5382271762</v>
       </c>
       <c r="I75" t="n">
-        <v>0.1627325992334198</v>
+        <v>0.1527549395839681</v>
       </c>
       <c r="J75" t="n">
-        <v>0.5996778058857872</v>
+        <v>0.6242228486234384</v>
       </c>
       <c r="K75" t="n">
-        <v>0.237589594880793</v>
+        <v>0.2230222117925935</v>
       </c>
       <c r="L75" t="n">
-        <v>0.7257873925810525</v>
+        <v>0.6812870305444978</v>
       </c>
       <c r="M75" t="n">
-        <v>2.036623012538155</v>
+        <v>2.095690757662909</v>
       </c>
       <c r="N75" t="n">
         <v>0</v>
@@ -3632,25 +3632,25 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="H76" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="I76" t="n">
-        <v>0.5829207016569499</v>
+        <v>0.6076399031241819</v>
       </c>
       <c r="J76" t="n">
-        <v>0.1695444302207521</v>
+        <v>0.1594959743397635</v>
       </c>
       <c r="K76" t="n">
-        <v>0.2475348681222981</v>
+        <v>0.2328641225360547</v>
       </c>
       <c r="L76" t="n">
-        <v>1.996296973093148</v>
+        <v>2.055783831908601</v>
       </c>
       <c r="M76" t="n">
-        <v>0.7561681587845545</v>
+        <v>0.7113520455553451</v>
       </c>
       <c r="N76" t="n">
         <v>3</v>
@@ -3763,25 +3763,25 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="H79" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="I79" t="n">
-        <v>0.3307468386004146</v>
+        <v>0.3192070317294386</v>
       </c>
       <c r="J79" t="n">
-        <v>0.2720541306502379</v>
+        <v>0.2767451090530738</v>
       </c>
       <c r="K79" t="n">
-        <v>0.3971990307493474</v>
+        <v>0.4040478592174876</v>
       </c>
       <c r="L79" t="n">
-        <v>1.389439546550591</v>
+        <v>1.361668954405803</v>
       </c>
       <c r="M79" t="n">
-        <v>1.213361422700061</v>
+        <v>1.234283186376709</v>
       </c>
       <c r="N79" t="n">
         <v>3</v>
@@ -4011,25 +4011,25 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="H85" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="I85" t="n">
-        <v>0.2899519337584784</v>
+        <v>0.2885454077379682</v>
       </c>
       <c r="J85" t="n">
-        <v>0.2886374253014315</v>
+        <v>0.2901782969645983</v>
       </c>
       <c r="K85" t="n">
-        <v>0.4214106409400901</v>
+        <v>0.4212762952974336</v>
       </c>
       <c r="L85" t="n">
-        <v>1.291266442215525</v>
+        <v>1.286912518511338</v>
       </c>
       <c r="M85" t="n">
-        <v>1.287322916844385</v>
+        <v>1.291811186191228</v>
       </c>
       <c r="N85" t="n">
         <v>3</v>
@@ -4064,25 +4064,25 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="H86" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="I86" t="n">
-        <v>0.6148244287988239</v>
+        <v>0.6315008501418395</v>
       </c>
       <c r="J86" t="n">
-        <v>0.1565754354476326</v>
+        <v>0.149796402381366</v>
       </c>
       <c r="K86" t="n">
-        <v>0.2286001357535435</v>
+        <v>0.2187027474767944</v>
       </c>
       <c r="L86" t="n">
-        <v>2.073073422150015</v>
+        <v>2.113205297902313</v>
       </c>
       <c r="M86" t="n">
-        <v>0.6983264420964412</v>
+        <v>0.6680919546208924</v>
       </c>
       <c r="N86" t="n">
         <v>0</v>
@@ -4312,25 +4312,25 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="H92" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="I92" t="n">
-        <v>0.6864185119515442</v>
+        <v>0.7002374869336235</v>
       </c>
       <c r="J92" t="n">
-        <v>0.1274721496131934</v>
+        <v>0.1218546801082831</v>
       </c>
       <c r="K92" t="n">
-        <v>0.1861093384352623</v>
+        <v>0.1779078329580934</v>
       </c>
       <c r="L92" t="n">
-        <v>2.245364874289895</v>
+        <v>2.278620293758964</v>
       </c>
       <c r="M92" t="n">
-        <v>0.5685257872748425</v>
+        <v>0.5434718732829428</v>
       </c>
       <c r="N92" t="n">
         <v>3</v>
@@ -4443,25 +4443,25 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="H95" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="I95" t="n">
-        <v>0.3279017101045909</v>
+        <v>0.2927790476367478</v>
       </c>
       <c r="J95" t="n">
-        <v>0.2732106869493533</v>
+        <v>0.2874881920175822</v>
       </c>
       <c r="K95" t="n">
-        <v>0.3988876029460558</v>
+        <v>0.41973276034567</v>
       </c>
       <c r="L95" t="n">
-        <v>1.382592733259828</v>
+        <v>1.298069903255914</v>
       </c>
       <c r="M95" t="n">
-        <v>1.218519663794116</v>
+        <v>1.282197336398416</v>
       </c>
       <c r="N95" t="n">
         <v>0</v>
@@ -4769,25 +4769,25 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="H103" t="n">
-        <v>96.88550713079999</v>
+        <v>97.0684976167</v>
       </c>
       <c r="I103" t="n">
-        <v>0.1815289569582933</v>
+        <v>0.1723817807031599</v>
       </c>
       <c r="J103" t="n">
-        <v>0.5534387658825987</v>
+        <v>0.5759408194702268</v>
       </c>
       <c r="K103" t="n">
-        <v>0.2650322771591082</v>
+        <v>0.2516773998266134</v>
       </c>
       <c r="L103" t="n">
-        <v>0.809619148033988</v>
+        <v>0.7688227419360929</v>
       </c>
       <c r="M103" t="n">
-        <v>1.925348574806904</v>
+        <v>1.979499858237294</v>
       </c>
       <c r="N103" t="n">
         <v>0</v>
@@ -5173,25 +5173,25 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="H113" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="I113" t="n">
-        <v>0.3994078930338434</v>
+        <v>0.3983373393883174</v>
       </c>
       <c r="J113" t="n">
-        <v>0.2441431329130717</v>
+        <v>0.2445783173218222</v>
       </c>
       <c r="K113" t="n">
-        <v>0.3564489740530847</v>
+        <v>0.3570843432898604</v>
       </c>
       <c r="L113" t="n">
-        <v>1.554672653154615</v>
+        <v>1.552096361454812</v>
       </c>
       <c r="M113" t="n">
-        <v>1.0888783727923</v>
+        <v>1.090819295255327</v>
       </c>
       <c r="N113" t="n">
         <v>0</v>
@@ -5343,25 +5343,25 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="H117" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="I117" t="n">
-        <v>0.4466259253308035</v>
+        <v>0.4693091807671989</v>
       </c>
       <c r="J117" t="n">
-        <v>0.2249488108411368</v>
+        <v>0.2157279752978866</v>
       </c>
       <c r="K117" t="n">
-        <v>0.3284252638280597</v>
+        <v>0.3149628439349144</v>
       </c>
       <c r="L117" t="n">
-        <v>1.66830303982047</v>
+        <v>1.722890386236511</v>
       </c>
       <c r="M117" t="n">
-        <v>1.00327169635147</v>
+        <v>0.9621467698285742</v>
       </c>
       <c r="N117" t="n">
         <v>1</v>
@@ -5474,25 +5474,25 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="H120" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="I120" t="n">
-        <v>0.406517025761056</v>
+        <v>0.3908238510763127</v>
       </c>
       <c r="J120" t="n">
-        <v>0.2412532415605464</v>
+        <v>0.2476325808632875</v>
       </c>
       <c r="K120" t="n">
-        <v>0.3522297326783977</v>
+        <v>0.3615435680603998</v>
       </c>
       <c r="L120" t="n">
-        <v>1.571780809961566</v>
+        <v>1.534015121289338</v>
       </c>
       <c r="M120" t="n">
-        <v>1.075989457360037</v>
+        <v>1.104441310650262</v>
       </c>
       <c r="N120" t="n">
         <v>3</v>
@@ -5722,25 +5722,25 @@
         </is>
       </c>
       <c r="G126" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="H126" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="I126" t="n">
-        <v>0.3322111342362393</v>
+        <v>0.3443704494738757</v>
       </c>
       <c r="J126" t="n">
-        <v>0.271458888521854</v>
+        <v>0.266516077449644</v>
       </c>
       <c r="K126" t="n">
-        <v>0.3963299772419068</v>
+        <v>0.3891134730764803</v>
       </c>
       <c r="L126" t="n">
-        <v>1.392963379950625</v>
+        <v>1.422224821498107</v>
       </c>
       <c r="M126" t="n">
-        <v>1.210706642807469</v>
+        <v>1.188661705425412</v>
       </c>
       <c r="N126" t="n">
         <v>1</v>
@@ -5814,25 +5814,25 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="H128" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="I128" t="n">
-        <v>0.5347798799137172</v>
+        <v>0.514280896366111</v>
       </c>
       <c r="J128" t="n">
-        <v>0.1891138699537735</v>
+        <v>0.1974467900950769</v>
       </c>
       <c r="K128" t="n">
-        <v>0.2761062501325093</v>
+        <v>0.2882723135388122</v>
       </c>
       <c r="L128" t="n">
-        <v>1.880445889873661</v>
+        <v>1.831115002637145</v>
       </c>
       <c r="M128" t="n">
-        <v>0.8434478599938298</v>
+        <v>0.8806126838240428</v>
       </c>
       <c r="N128" t="n">
         <v>3</v>
@@ -5945,25 +5945,25 @@
         </is>
       </c>
       <c r="G131" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="H131" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="I131" t="n">
-        <v>0.2500154823738698</v>
+        <v>0.2503868044526076</v>
       </c>
       <c r="J131" t="n">
-        <v>0.3849619133602801</v>
+        <v>0.3840484610465855</v>
       </c>
       <c r="K131" t="n">
-        <v>0.36502260426585</v>
+        <v>0.365564734500807</v>
       </c>
       <c r="L131" t="n">
-        <v>1.115069051387459</v>
+        <v>1.11672514785863</v>
       </c>
       <c r="M131" t="n">
-        <v>1.51990834434669</v>
+        <v>1.517710117640563</v>
       </c>
       <c r="N131" t="n">
         <v>1</v>
@@ -6310,25 +6310,25 @@
         </is>
       </c>
       <c r="G140" t="n">
-        <v>92.1163744242</v>
+        <v>91.5882912066</v>
       </c>
       <c r="H140" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="I140" t="n">
-        <v>0.6592686980829936</v>
+        <v>0.6598587972747965</v>
       </c>
       <c r="J140" t="n">
-        <v>0.1385086593158563</v>
+        <v>0.1382687815956112</v>
       </c>
       <c r="K140" t="n">
-        <v>0.2022226426011502</v>
+        <v>0.2018724211295923</v>
       </c>
       <c r="L140" t="n">
-        <v>2.180028736850131</v>
+        <v>2.181448812953982</v>
       </c>
       <c r="M140" t="n">
-        <v>0.617748620548719</v>
+        <v>0.6166787659164259</v>
       </c>
       <c r="N140" t="n">
         <v>3</v>
@@ -6558,25 +6558,25 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="H146" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="I146" t="n">
-        <v>0.4559047806525845</v>
+        <v>0.4455545059743875</v>
       </c>
       <c r="J146" t="n">
-        <v>0.2211769184339087</v>
+        <v>0.2253843471648831</v>
       </c>
       <c r="K146" t="n">
-        <v>0.3229183009135068</v>
+        <v>0.3290611468607294</v>
       </c>
       <c r="L146" t="n">
-        <v>1.69063264287126</v>
+        <v>1.665724664783892</v>
       </c>
       <c r="M146" t="n">
-        <v>0.986449056215233</v>
+        <v>1.005214188355379</v>
       </c>
       <c r="N146" t="n">
         <v>1</v>
@@ -6689,25 +6689,25 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="H149" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="I149" t="n">
-        <v>0.2996920680638719</v>
+        <v>0.2954822796927676</v>
       </c>
       <c r="J149" t="n">
-        <v>0.2846780211122472</v>
+        <v>0.2863893171980619</v>
       </c>
       <c r="K149" t="n">
-        <v>0.415629910823881</v>
+        <v>0.4181284031091704</v>
       </c>
       <c r="L149" t="n">
-        <v>1.314706115015497</v>
+        <v>1.304575242187473</v>
       </c>
       <c r="M149" t="n">
-        <v>1.269663974160623</v>
+        <v>1.277296354703356</v>
       </c>
       <c r="N149" t="n">
         <v>3</v>
@@ -6742,25 +6742,25 @@
         </is>
       </c>
       <c r="G150" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="H150" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="I150" t="n">
-        <v>0.4929741783903543</v>
+        <v>0.489605858383666</v>
       </c>
       <c r="J150" t="n">
-        <v>0.2061080575648966</v>
+        <v>0.2074772933399732</v>
       </c>
       <c r="K150" t="n">
-        <v>0.3009177640447491</v>
+        <v>0.3029168482763608</v>
       </c>
       <c r="L150" t="n">
-        <v>1.779840299215812</v>
+        <v>1.771734423427359</v>
       </c>
       <c r="M150" t="n">
-        <v>0.9192419367394391</v>
+        <v>0.9253487282962805</v>
       </c>
       <c r="N150" t="n">
         <v>0</v>
@@ -7068,25 +7068,25 @@
         </is>
       </c>
       <c r="G158" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="H158" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="I158" t="n">
-        <v>0.62001741204529</v>
+        <v>0.6128735115879784</v>
       </c>
       <c r="J158" t="n">
-        <v>0.154464466648256</v>
+        <v>0.1573684912243991</v>
       </c>
       <c r="K158" t="n">
-        <v>0.2255181213064538</v>
+        <v>0.2297579971876226</v>
       </c>
       <c r="L158" t="n">
-        <v>2.085570357442324</v>
+        <v>2.068378531951558</v>
       </c>
       <c r="M158" t="n">
-        <v>0.6889115212512219</v>
+        <v>0.7018634708608198</v>
       </c>
       <c r="N158" t="n">
         <v>3</v>
@@ -7277,25 +7277,25 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="H163" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="I163" t="n">
-        <v>0.2975504800847637</v>
+        <v>0.2868616074327283</v>
       </c>
       <c r="J163" t="n">
-        <v>0.2855485853313969</v>
+        <v>0.2943204457154883</v>
       </c>
       <c r="K163" t="n">
-        <v>0.4169009345838394</v>
+        <v>0.4188179468517833</v>
       </c>
       <c r="L163" t="n">
-        <v>1.309552374838131</v>
+        <v>1.279402769149968</v>
       </c>
       <c r="M163" t="n">
-        <v>1.27354669057803</v>
+        <v>1.301779283998248</v>
       </c>
       <c r="N163" t="n">
         <v>1</v>
@@ -7447,25 +7447,25 @@
         </is>
       </c>
       <c r="G167" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="H167" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="I167" t="n">
-        <v>0.2415656968122777</v>
+        <v>0.2380990410465822</v>
       </c>
       <c r="J167" t="n">
-        <v>0.4057483858417969</v>
+        <v>0.4142763590254078</v>
       </c>
       <c r="K167" t="n">
-        <v>0.3526859173459254</v>
+        <v>0.3476245999280101</v>
       </c>
       <c r="L167" t="n">
-        <v>1.077383007782758</v>
+        <v>1.061921723067757</v>
       </c>
       <c r="M167" t="n">
-        <v>1.569931074871316</v>
+        <v>1.590453677004233</v>
       </c>
       <c r="N167" t="n">
         <v>0</v>
@@ -7539,25 +7539,25 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="H169" t="n">
-        <v>94.474011971</v>
+        <v>94.2958640271</v>
       </c>
       <c r="I169" t="n">
-        <v>0.2156711958689996</v>
+        <v>0.2256337788840803</v>
       </c>
       <c r="J169" t="n">
-        <v>0.4694488581622608</v>
+        <v>0.4449409039451626</v>
       </c>
       <c r="K169" t="n">
-        <v>0.3148799459687395</v>
+        <v>0.3294253171707572</v>
       </c>
       <c r="L169" t="n">
-        <v>0.9618935335757384</v>
+        <v>1.006326653822998</v>
       </c>
       <c r="M169" t="n">
-        <v>1.723226520455522</v>
+        <v>1.664248029006245</v>
       </c>
       <c r="N169" t="n">
         <v>0</v>
@@ -7943,25 +7943,25 @@
         </is>
       </c>
       <c r="G179" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="H179" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="I179" t="n">
-        <v>0.4167425297508313</v>
+        <v>0.4322105110685806</v>
       </c>
       <c r="J179" t="n">
-        <v>0.2370965326216133</v>
+        <v>0.2308087353379754</v>
       </c>
       <c r="K179" t="n">
-        <v>0.3461609376275554</v>
+        <v>0.336980753593444</v>
       </c>
       <c r="L179" t="n">
-        <v>1.596388526880049</v>
+        <v>1.633612286799186</v>
       </c>
       <c r="M179" t="n">
-        <v>1.057450535492395</v>
+        <v>1.02940695960737</v>
       </c>
       <c r="N179" t="n">
         <v>1</v>
@@ -7996,25 +7996,25 @@
         </is>
       </c>
       <c r="G180" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="H180" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="I180" t="n">
-        <v>0.3445411679560992</v>
+        <v>0.3438662235128096</v>
       </c>
       <c r="J180" t="n">
-        <v>0.2664466796926426</v>
+        <v>0.2667210473525164</v>
       </c>
       <c r="K180" t="n">
-        <v>0.3890121523512582</v>
+        <v>0.3894127291346739</v>
       </c>
       <c r="L180" t="n">
-        <v>1.422635656219556</v>
+        <v>1.421011399673103</v>
       </c>
       <c r="M180" t="n">
-        <v>1.188352191429186</v>
+        <v>1.189575871192223</v>
       </c>
       <c r="N180" t="n">
         <v>0</v>
@@ -8361,25 +8361,25 @@
         </is>
       </c>
       <c r="G189" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="H189" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="I189" t="n">
-        <v>0.2531637771732934</v>
+        <v>0.2536649429911881</v>
       </c>
       <c r="J189" t="n">
-        <v>0.3772171081536982</v>
+        <v>0.3759842402416773</v>
       </c>
       <c r="K189" t="n">
-        <v>0.3696191146730083</v>
+        <v>0.3703508167671345</v>
       </c>
       <c r="L189" t="n">
-        <v>1.129110446192889</v>
+        <v>1.131345645740699</v>
       </c>
       <c r="M189" t="n">
-        <v>1.501270439134103</v>
+        <v>1.498303537492166</v>
       </c>
       <c r="N189" t="n">
         <v>1</v>
@@ -8492,25 +8492,25 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="H192" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="I192" t="n">
-        <v>0.6259689423692113</v>
+        <v>0.6219789617313686</v>
       </c>
       <c r="J192" t="n">
-        <v>0.1520451453783694</v>
+        <v>0.153667088727086</v>
       </c>
       <c r="K192" t="n">
-        <v>0.2219859122524193</v>
+        <v>0.2243539495415456</v>
       </c>
       <c r="L192" t="n">
-        <v>2.099892739360053</v>
+        <v>2.090290834735651</v>
       </c>
       <c r="M192" t="n">
-        <v>0.6781213483875275</v>
+        <v>0.6853552157228034</v>
       </c>
       <c r="N192" t="n">
         <v>3</v>
@@ -8701,25 +8701,25 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="H197" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="I197" t="n">
-        <v>0.2522672277823765</v>
+        <v>0.2663581849888516</v>
       </c>
       <c r="J197" t="n">
-        <v>0.3794226196553538</v>
+        <v>0.3447588649274251</v>
       </c>
       <c r="K197" t="n">
-        <v>0.3683101525622697</v>
+        <v>0.3888829500837234</v>
       </c>
       <c r="L197" t="n">
-        <v>1.125111835909399</v>
+        <v>1.187957505050278</v>
       </c>
       <c r="M197" t="n">
-        <v>1.506578011528331</v>
+        <v>1.423159544865999</v>
       </c>
       <c r="N197" t="n">
         <v>0</v>
@@ -8754,25 +8754,25 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>91.8865135193</v>
+        <v>91.34868924840001</v>
       </c>
       <c r="H198" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="I198" t="n">
-        <v>0.6515560928528449</v>
+        <v>0.6518241230244103</v>
       </c>
       <c r="J198" t="n">
-        <v>0.1416438646939654</v>
+        <v>0.1415349093396706</v>
       </c>
       <c r="K198" t="n">
-        <v>0.2068000424531896</v>
+        <v>0.2066409676359191</v>
       </c>
       <c r="L198" t="n">
-        <v>2.161468321011724</v>
+        <v>2.16211333670915</v>
       </c>
       <c r="M198" t="n">
-        <v>0.6317316365350859</v>
+        <v>0.6312456956549309</v>
       </c>
       <c r="N198" t="n">
         <v>1</v>
@@ -8885,25 +8885,25 @@
         </is>
       </c>
       <c r="G201" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="H201" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="I201" t="n">
-        <v>0.6568425428953005</v>
+        <v>0.6696268093148474</v>
       </c>
       <c r="J201" t="n">
-        <v>0.139494901262073</v>
+        <v>0.1342980449939645</v>
       </c>
       <c r="K201" t="n">
-        <v>0.2036625558426265</v>
+        <v>0.1960751456911881</v>
       </c>
       <c r="L201" t="n">
-        <v>2.174190184528528</v>
+        <v>2.20495557363573</v>
       </c>
       <c r="M201" t="n">
-        <v>0.6221472596288453</v>
+        <v>0.5989692806730815</v>
       </c>
       <c r="N201" t="n">
         <v>1</v>
@@ -8977,25 +8977,25 @@
         </is>
       </c>
       <c r="G203" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="H203" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="I203" t="n">
-        <v>0.5870075790755178</v>
+        <v>0.5859643731818495</v>
       </c>
       <c r="J203" t="n">
-        <v>0.1678830979367814</v>
+        <v>0.168307165373232</v>
       </c>
       <c r="K203" t="n">
-        <v>0.2451093229877008</v>
+        <v>0.2457284614449186</v>
       </c>
       <c r="L203" t="n">
-        <v>2.006132060214254</v>
+        <v>2.003621580990467</v>
       </c>
       <c r="M203" t="n">
-        <v>0.748758616798045</v>
+        <v>0.7506499575646145</v>
       </c>
       <c r="N203" t="n">
         <v>1</v>
@@ -9108,25 +9108,25 @@
         </is>
       </c>
       <c r="G206" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="H206" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="I206" t="n">
-        <v>0.2328412264746729</v>
+        <v>0.2362121888262549</v>
       </c>
       <c r="J206" t="n">
-        <v>0.4272105828723047</v>
+        <v>0.418918015487413</v>
       </c>
       <c r="K206" t="n">
-        <v>0.3399481906530225</v>
+        <v>0.3448697956863322</v>
       </c>
       <c r="L206" t="n">
-        <v>1.038471870077041</v>
+        <v>1.053506362165097</v>
       </c>
       <c r="M206" t="n">
-        <v>1.621579939269936</v>
+        <v>1.601623842148571</v>
       </c>
       <c r="N206" t="n">
         <v>1</v>
@@ -9512,25 +9512,25 @@
         </is>
       </c>
       <c r="G216" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="H216" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="I216" t="n">
-        <v>0.2690060694644226</v>
+        <v>0.2731421635021063</v>
       </c>
       <c r="J216" t="n">
-        <v>0.3382450691175204</v>
+        <v>0.3280702777848187</v>
       </c>
       <c r="K216" t="n">
-        <v>0.3927488614180569</v>
+        <v>0.3987875587130751</v>
       </c>
       <c r="L216" t="n">
-        <v>1.199767069811325</v>
+        <v>1.218214049219394</v>
       </c>
       <c r="M216" t="n">
-        <v>1.407484068770618</v>
+        <v>1.382998392067531</v>
       </c>
       <c r="N216" t="n">
         <v>3</v>
@@ -9643,25 +9643,25 @@
         </is>
       </c>
       <c r="G219" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="H219" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="I219" t="n">
-        <v>0.3846103619385959</v>
+        <v>0.3789158351703988</v>
       </c>
       <c r="J219" t="n">
-        <v>0.2501583894558553</v>
+        <v>0.2524732377356102</v>
       </c>
       <c r="K219" t="n">
-        <v>0.3652312486055487</v>
+        <v>0.3686109270939909</v>
       </c>
       <c r="L219" t="n">
-        <v>1.519062334421337</v>
+        <v>1.505358432605187</v>
       </c>
       <c r="M219" t="n">
-        <v>1.115706416973115</v>
+        <v>1.126030640300821</v>
       </c>
       <c r="N219" t="n">
         <v>3</v>
@@ -9735,25 +9735,25 @@
         </is>
       </c>
       <c r="G221" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="H221" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="I221" t="n">
-        <v>0.4456209434253541</v>
+        <v>0.4408294825740331</v>
       </c>
       <c r="J221" t="n">
-        <v>0.2253573400709942</v>
+        <v>0.2273050883845394</v>
       </c>
       <c r="K221" t="n">
-        <v>0.3290217165036516</v>
+        <v>0.3318654290414275</v>
       </c>
       <c r="L221" t="n">
-        <v>1.665884546779714</v>
+        <v>1.654353876763527</v>
       </c>
       <c r="M221" t="n">
-        <v>1.005093736716634</v>
+        <v>1.013780694195046</v>
       </c>
       <c r="N221" t="n">
         <v>0</v>
@@ -9788,25 +9788,25 @@
         </is>
       </c>
       <c r="G222" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="H222" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="I222" t="n">
-        <v>0.4153914577162995</v>
+        <v>0.3881329752501469</v>
       </c>
       <c r="J222" t="n">
-        <v>0.2376457488958132</v>
+        <v>0.2487264328251435</v>
       </c>
       <c r="K222" t="n">
-        <v>0.3469627933878872</v>
+        <v>0.3631405919247096</v>
       </c>
       <c r="L222" t="n">
-        <v>1.593137166536786</v>
+        <v>1.52753951767515</v>
       </c>
       <c r="M222" t="n">
-        <v>1.059900040075327</v>
+        <v>1.10931989040014</v>
       </c>
       <c r="N222" t="n">
         <v>3</v>
@@ -9880,25 +9880,25 @@
         </is>
       </c>
       <c r="G224" t="n">
-        <v>86.0714001091</v>
+        <v>85.7823829526</v>
       </c>
       <c r="H224" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="I224" t="n">
-        <v>0.4407611662867085</v>
+        <v>0.4501840594900287</v>
       </c>
       <c r="J224" t="n">
-        <v>0.2273328592330453</v>
+        <v>0.2235024148414517</v>
       </c>
       <c r="K224" t="n">
-        <v>0.3319059744802461</v>
+        <v>0.3263135256685195</v>
       </c>
       <c r="L224" t="n">
-        <v>1.654189473340372</v>
+        <v>1.676865704138605</v>
       </c>
       <c r="M224" t="n">
-        <v>1.013904552179382</v>
+        <v>0.9968207701928746</v>
       </c>
       <c r="N224" t="n">
         <v>1</v>
@@ -10167,25 +10167,25 @@
         </is>
       </c>
       <c r="G231" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="H231" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="I231" t="n">
-        <v>0.4298357726227335</v>
+        <v>0.4066445905697262</v>
       </c>
       <c r="J231" t="n">
-        <v>0.2317740761696206</v>
+        <v>0.2412013859472658</v>
       </c>
       <c r="K231" t="n">
-        <v>0.338390151207646</v>
+        <v>0.352154023483008</v>
       </c>
       <c r="L231" t="n">
-        <v>1.627897469075846</v>
+        <v>1.572087795192187</v>
       </c>
       <c r="M231" t="n">
-        <v>1.033712379716508</v>
+        <v>1.075758181324805</v>
       </c>
       <c r="N231" t="n">
         <v>0</v>
@@ -10259,25 +10259,25 @@
         </is>
       </c>
       <c r="G233" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="H233" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="I233" t="n">
-        <v>0.2810510673871032</v>
+        <v>0.2762605153417524</v>
       </c>
       <c r="J233" t="n">
-        <v>0.3086143742277263</v>
+        <v>0.320399132259289</v>
       </c>
       <c r="K233" t="n">
-        <v>0.4103345583851706</v>
+        <v>0.4033403523989585</v>
       </c>
       <c r="L233" t="n">
-        <v>1.25348776054648</v>
+        <v>1.232121898424216</v>
       </c>
       <c r="M233" t="n">
-        <v>1.336177681068349</v>
+        <v>1.364537749176825</v>
       </c>
       <c r="N233" t="n">
         <v>3</v>
@@ -10702,25 +10702,25 @@
         </is>
       </c>
       <c r="G244" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="H244" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="I244" t="n">
-        <v>0.6145824263287731</v>
+        <v>0.6320310560431134</v>
       </c>
       <c r="J244" t="n">
-        <v>0.1566738104354581</v>
+        <v>0.1495808715271897</v>
       </c>
       <c r="K244" t="n">
-        <v>0.2287437632357688</v>
+        <v>0.218388072429697</v>
       </c>
       <c r="L244" t="n">
-        <v>2.072491042222088</v>
+        <v>2.114481240559037</v>
       </c>
       <c r="M244" t="n">
-        <v>0.698765194542143</v>
+        <v>0.6671306870112662</v>
       </c>
       <c r="N244" t="n">
         <v>1</v>
@@ -10833,25 +10833,25 @@
         </is>
       </c>
       <c r="G247" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="H247" t="n">
-        <v>93.1897250565</v>
+        <v>93.29711155859999</v>
       </c>
       <c r="I247" t="n">
-        <v>0.2340919691644765</v>
+        <v>0.2398223198409242</v>
       </c>
       <c r="J247" t="n">
-        <v>0.4241337558553877</v>
+        <v>0.4100370931913264</v>
       </c>
       <c r="K247" t="n">
-        <v>0.3417742749801357</v>
+        <v>0.3501405869677494</v>
       </c>
       <c r="L247" t="n">
-        <v>1.044050182473565</v>
+        <v>1.069607546490522</v>
       </c>
       <c r="M247" t="n">
-        <v>1.614175542546299</v>
+        <v>1.580251866541728</v>
       </c>
       <c r="N247" t="n">
         <v>0</v>
@@ -11315,25 +11315,25 @@
         </is>
       </c>
       <c r="G259" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="H259" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="I259" t="n">
-        <v>0.315491125078724</v>
+        <v>0.3258890827284512</v>
       </c>
       <c r="J259" t="n">
-        <v>0.2782556402119009</v>
+        <v>0.2740288281591662</v>
       </c>
       <c r="K259" t="n">
-        <v>0.4062532347093752</v>
+        <v>0.4000820891123826</v>
       </c>
       <c r="L259" t="n">
-        <v>1.352726609945547</v>
+        <v>1.377749337297736</v>
       </c>
       <c r="M259" t="n">
-        <v>1.241020155345078</v>
+        <v>1.222168573589881</v>
       </c>
       <c r="N259" t="n">
         <v>1</v>
@@ -11485,25 +11485,25 @@
         </is>
       </c>
       <c r="G263" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="H263" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="I263" t="n">
-        <v>0.403880624464345</v>
+        <v>0.3922710341012632</v>
       </c>
       <c r="J263" t="n">
-        <v>0.2423249494047378</v>
+        <v>0.2470442950807873</v>
       </c>
       <c r="K263" t="n">
-        <v>0.3537944261309172</v>
+        <v>0.3606846708179495</v>
       </c>
       <c r="L263" t="n">
-        <v>1.565436299523952</v>
+        <v>1.537497773121739</v>
       </c>
       <c r="M263" t="n">
-        <v>1.080769274345131</v>
+        <v>1.101817556060312</v>
       </c>
       <c r="N263" t="n">
         <v>3</v>
@@ -11577,25 +11577,25 @@
         </is>
       </c>
       <c r="G265" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="H265" t="n">
-        <v>91.1863355645</v>
+        <v>90.8794818878</v>
       </c>
       <c r="I265" t="n">
-        <v>0.2624240391314183</v>
+        <v>0.2604106175185235</v>
       </c>
       <c r="J265" t="n">
-        <v>0.3544368637367111</v>
+        <v>0.359389880904432</v>
       </c>
       <c r="K265" t="n">
-        <v>0.3831390971318706</v>
+        <v>0.3801995015770444</v>
       </c>
       <c r="L265" t="n">
-        <v>1.170411214526125</v>
+        <v>1.161431354132615</v>
       </c>
       <c r="M265" t="n">
-        <v>1.446449688342004</v>
+        <v>1.45836914429034</v>
       </c>
       <c r="N265" t="n">
         <v>0</v>
@@ -11981,25 +11981,25 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="H275" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="I275" t="n">
-        <v>0.3004864879548296</v>
+        <v>0.2949800901788114</v>
       </c>
       <c r="J275" t="n">
-        <v>0.2843550861972237</v>
+        <v>0.2865934592769059</v>
       </c>
       <c r="K275" t="n">
-        <v>0.4151584258479466</v>
+        <v>0.4184264505442826</v>
       </c>
       <c r="L275" t="n">
-        <v>1.316617889712435</v>
+        <v>1.303366721080717</v>
       </c>
       <c r="M275" t="n">
-        <v>1.268223684439618</v>
+        <v>1.278206828375001</v>
       </c>
       <c r="N275" t="n">
         <v>3</v>
@@ -12034,25 +12034,25 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="H276" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="I276" t="n">
-        <v>0.333273449921293</v>
+        <v>0.3602809187492645</v>
       </c>
       <c r="J276" t="n">
-        <v>0.2710270528775232</v>
+        <v>0.2600484070124941</v>
       </c>
       <c r="K276" t="n">
-        <v>0.3956994972011838</v>
+        <v>0.3796706742382414</v>
       </c>
       <c r="L276" t="n">
-        <v>1.395519846965063</v>
+        <v>1.460513430486035</v>
       </c>
       <c r="M276" t="n">
-        <v>1.208780655833753</v>
+        <v>1.159815895275724</v>
       </c>
       <c r="N276" t="n">
         <v>3</v>
@@ -12126,25 +12126,25 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="H278" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="I278" t="n">
-        <v>0.5359700601172617</v>
+        <v>0.5316755208620507</v>
       </c>
       <c r="J278" t="n">
-        <v>0.1886300568629018</v>
+        <v>0.1903758045276217</v>
       </c>
       <c r="K278" t="n">
-        <v>0.2753998830198366</v>
+        <v>0.2779486746103276</v>
       </c>
       <c r="L278" t="n">
-        <v>1.883310063371622</v>
+        <v>1.87297523719648</v>
       </c>
       <c r="M278" t="n">
-        <v>0.8412900536085419</v>
+        <v>0.8490760881931927</v>
       </c>
       <c r="N278" t="n">
         <v>1</v>
@@ -12647,25 +12647,25 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="H291" t="n">
-        <v>92.14857895439999</v>
+        <v>92.0576470387</v>
       </c>
       <c r="I291" t="n">
-        <v>0.2381437594452739</v>
+        <v>0.2310671529824628</v>
       </c>
       <c r="J291" t="n">
-        <v>0.4141663517646261</v>
+        <v>0.4315748036631415</v>
       </c>
       <c r="K291" t="n">
-        <v>0.3476898887900999</v>
+        <v>0.3373580433543957</v>
       </c>
       <c r="L291" t="n">
-        <v>1.062121167125922</v>
+        <v>1.030559502301784</v>
       </c>
       <c r="M291" t="n">
-        <v>1.590188944083978</v>
+        <v>1.63208245434382</v>
       </c>
       <c r="N291" t="n">
         <v>1</v>
@@ -12739,25 +12739,25 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="H293" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="I293" t="n">
-        <v>0.273842507069197</v>
+        <v>0.2771795870100657</v>
       </c>
       <c r="J293" t="n">
-        <v>0.3263474326097753</v>
+        <v>0.3181382159552383</v>
       </c>
       <c r="K293" t="n">
-        <v>0.3998100603210276</v>
+        <v>0.4046821970346959</v>
       </c>
       <c r="L293" t="n">
-        <v>1.221337581528619</v>
+        <v>1.236220958064893</v>
       </c>
       <c r="M293" t="n">
-        <v>1.378852358150354</v>
+        <v>1.359096844900411</v>
       </c>
       <c r="N293" t="n">
         <v>1</v>
@@ -12792,25 +12792,25 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="H294" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="I294" t="n">
-        <v>0.3885040601458871</v>
+        <v>0.4011165254580791</v>
       </c>
       <c r="J294" t="n">
-        <v>0.24857558530655</v>
+        <v>0.2434485668869597</v>
       </c>
       <c r="K294" t="n">
-        <v>0.3629203545475629</v>
+        <v>0.3554349076549612</v>
       </c>
       <c r="L294" t="n">
-        <v>1.528432534985224</v>
+        <v>1.558784484029199</v>
       </c>
       <c r="M294" t="n">
-        <v>1.108647110467213</v>
+        <v>1.085780608315841</v>
       </c>
       <c r="N294" t="n">
         <v>1</v>
@@ -12884,25 +12884,25 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="H296" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="I296" t="n">
-        <v>0.5948233194042617</v>
+        <v>0.5744918982960001</v>
       </c>
       <c r="J296" t="n">
-        <v>0.1647059677218449</v>
+        <v>0.1729707730504064</v>
       </c>
       <c r="K296" t="n">
-        <v>0.2404707128738935</v>
+        <v>0.2525373286535934</v>
       </c>
       <c r="L296" t="n">
-        <v>2.024940671086679</v>
+        <v>1.976013023541594</v>
       </c>
       <c r="M296" t="n">
-        <v>0.7345886160394282</v>
+        <v>0.7714496478048126</v>
       </c>
       <c r="N296" t="n">
         <v>3</v>
@@ -13093,25 +13093,25 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="H301" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="I301" t="n">
-        <v>0.3192168078172902</v>
+        <v>0.3158847921802971</v>
       </c>
       <c r="J301" t="n">
-        <v>0.2767411350336219</v>
+        <v>0.2780956129348386</v>
       </c>
       <c r="K301" t="n">
-        <v>0.404042057149088</v>
+        <v>0.4060195948848643</v>
       </c>
       <c r="L301" t="n">
-        <v>1.361692480600959</v>
+        <v>1.353673971425756</v>
       </c>
       <c r="M301" t="n">
-        <v>1.234265462249954</v>
+        <v>1.24030643368938</v>
       </c>
       <c r="N301" t="n">
         <v>3</v>
@@ -13146,25 +13146,25 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>93.76269800439999</v>
+        <v>93.2242913626</v>
       </c>
       <c r="H302" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="I302" t="n">
-        <v>0.6886272403231403</v>
+        <v>0.6849506078353624</v>
       </c>
       <c r="J302" t="n">
-        <v>0.126574292551569</v>
+        <v>0.1280688586035112</v>
       </c>
       <c r="K302" t="n">
-        <v>0.1847984671252907</v>
+        <v>0.1869805335611264</v>
       </c>
       <c r="L302" t="n">
-        <v>2.250680188094711</v>
+        <v>2.241832357067214</v>
       </c>
       <c r="M302" t="n">
-        <v>0.5645213447799977</v>
+        <v>0.5711871093716602</v>
       </c>
       <c r="N302" t="n">
         <v>3</v>
@@ -13667,25 +13667,25 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="H315" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="I315" t="n">
-        <v>0.2925297024238229</v>
+        <v>0.2876145115562011</v>
       </c>
       <c r="J315" t="n">
-        <v>0.2875895518602346</v>
+        <v>0.2924683015717454</v>
       </c>
       <c r="K315" t="n">
-        <v>0.4198807457159425</v>
+        <v>0.4199171868720536</v>
       </c>
       <c r="L315" t="n">
-        <v>1.297469852987411</v>
+        <v>1.282760721540657</v>
       </c>
       <c r="M315" t="n">
-        <v>1.282649401296646</v>
+        <v>1.29732209158729</v>
       </c>
       <c r="N315" t="n">
         <v>3</v>
@@ -13954,25 +13954,25 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="H322" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="I322" t="n">
-        <v>0.5224323668326576</v>
+        <v>0.4949895287024574</v>
       </c>
       <c r="J322" t="n">
-        <v>0.1941331842143668</v>
+        <v>0.2052888094705458</v>
       </c>
       <c r="K322" t="n">
-        <v>0.2834344489529755</v>
+        <v>0.2997216618269969</v>
       </c>
       <c r="L322" t="n">
-        <v>1.850731549450948</v>
+        <v>1.784690247934369</v>
       </c>
       <c r="M322" t="n">
-        <v>0.8658340015960759</v>
+        <v>0.9155880902386342</v>
       </c>
       <c r="N322" t="n">
         <v>1</v>
@@ -14085,25 +14085,25 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="H325" t="n">
-        <v>88.9758001383</v>
+        <v>88.7111050262</v>
       </c>
       <c r="I325" t="n">
-        <v>0.2804793687189682</v>
+        <v>0.2763992781371433</v>
       </c>
       <c r="J325" t="n">
-        <v>0.3100207529513382</v>
+        <v>0.3200577757826273</v>
       </c>
       <c r="K325" t="n">
-        <v>0.4094998783296935</v>
+        <v>0.4035429460802293</v>
       </c>
       <c r="L325" t="n">
-        <v>1.250937984486598</v>
+        <v>1.232740780491659</v>
       </c>
       <c r="M325" t="n">
-        <v>1.339562137183708</v>
+        <v>1.363716273428111</v>
       </c>
       <c r="N325" t="n">
         <v>1</v>
@@ -14255,25 +14255,25 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="H329" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="I329" t="n">
-        <v>0.217873127899569</v>
+        <v>0.2240450199925548</v>
       </c>
       <c r="J329" t="n">
-        <v>0.4640321053670604</v>
+        <v>0.4488492508183153</v>
       </c>
       <c r="K329" t="n">
-        <v>0.3180947667333707</v>
+        <v>0.3271057291891299</v>
       </c>
       <c r="L329" t="n">
-        <v>0.9717141504320779</v>
+        <v>0.9992407891667943</v>
       </c>
       <c r="M329" t="n">
-        <v>1.710191082834552</v>
+        <v>1.673653481644076</v>
       </c>
       <c r="N329" t="n">
         <v>1</v>
@@ -14464,25 +14464,25 @@
         </is>
       </c>
       <c r="G334" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="H334" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="I334" t="n">
-        <v>0.6557795780717348</v>
+        <v>0.6375669461605379</v>
       </c>
       <c r="J334" t="n">
-        <v>0.1399270007838476</v>
+        <v>0.1473305096908382</v>
       </c>
       <c r="K334" t="n">
-        <v>0.2042934211444176</v>
+        <v>0.2151025441486238</v>
       </c>
       <c r="L334" t="n">
-        <v>2.171632155359622</v>
+        <v>2.127803382630237</v>
       </c>
       <c r="M334" t="n">
-        <v>0.6240744234959605</v>
+        <v>0.6570940732211386</v>
       </c>
       <c r="N334" t="n">
         <v>3</v>
@@ -14634,25 +14634,25 @@
         </is>
       </c>
       <c r="G338" t="n">
-        <v>94.3873093391</v>
+        <v>93.4578390827</v>
       </c>
       <c r="H338" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="I338" t="n">
-        <v>0.7305535836770592</v>
+        <v>0.7191857870111618</v>
       </c>
       <c r="J338" t="n">
-        <v>0.1095310635459109</v>
+        <v>0.1141521191011537</v>
       </c>
       <c r="K338" t="n">
-        <v>0.1599153527770299</v>
+        <v>0.1666620938876844</v>
       </c>
       <c r="L338" t="n">
-        <v>2.351576103808208</v>
+        <v>2.32421945492117</v>
       </c>
       <c r="M338" t="n">
-        <v>0.4885085434147625</v>
+        <v>0.5091184511911456</v>
       </c>
       <c r="N338" t="n">
         <v>3</v>
@@ -14726,25 +14726,25 @@
         </is>
       </c>
       <c r="G340" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="H340" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="I340" t="n">
-        <v>0.503430171517531</v>
+        <v>0.5215979884453531</v>
       </c>
       <c r="J340" t="n">
-        <v>0.2018576538546622</v>
+        <v>0.1944723624205882</v>
       </c>
       <c r="K340" t="n">
-        <v>0.2947121746278067</v>
+        <v>0.2839296491340587</v>
       </c>
       <c r="L340" t="n">
-        <v>1.8050026891804</v>
+        <v>1.848723614470118</v>
       </c>
       <c r="M340" t="n">
-        <v>0.9002851361917933</v>
+        <v>0.8673467363958232</v>
       </c>
       <c r="N340" t="n">
         <v>3</v>
@@ -14818,25 +14818,25 @@
         </is>
       </c>
       <c r="G342" t="n">
-        <v>88.5244880826</v>
+        <v>88.55071952030001</v>
       </c>
       <c r="H342" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="I342" t="n">
-        <v>0.3176181957769281</v>
+        <v>0.3380265351162132</v>
       </c>
       <c r="J342" t="n">
-        <v>0.277390977326452</v>
+        <v>0.2690949044243036</v>
       </c>
       <c r="K342" t="n">
-        <v>0.4049908268966199</v>
+        <v>0.3928785604594832</v>
       </c>
       <c r="L342" t="n">
-        <v>1.357845414227404</v>
+        <v>1.406958165808123</v>
       </c>
       <c r="M342" t="n">
-        <v>1.237163758875976</v>
+        <v>1.200163273732394</v>
       </c>
       <c r="N342" t="n">
         <v>3</v>
@@ -15339,25 +15339,25 @@
         </is>
       </c>
       <c r="G355" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="H355" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="I355" t="n">
-        <v>0.398327689473156</v>
+        <v>0.399145652288129</v>
       </c>
       <c r="J355" t="n">
-        <v>0.2445822400515626</v>
+        <v>0.244249734842224</v>
       </c>
       <c r="K355" t="n">
-        <v>0.3570900704752814</v>
+        <v>0.356604612869647</v>
       </c>
       <c r="L355" t="n">
-        <v>1.55207313889475</v>
+        <v>1.554041569734034</v>
       </c>
       <c r="M355" t="n">
-        <v>1.090836790629969</v>
+        <v>1.089353817396319</v>
       </c>
       <c r="N355" t="n">
         <v>3</v>
@@ -15587,25 +15587,25 @@
         </is>
       </c>
       <c r="G361" t="n">
-        <v>84.8796410094</v>
+        <v>84.31203815969999</v>
       </c>
       <c r="H361" t="n">
-        <v>85.66829184700001</v>
+        <v>85.1864986245</v>
       </c>
       <c r="I361" t="n">
-        <v>0.3710303275712374</v>
+        <v>0.3674199741191175</v>
       </c>
       <c r="J361" t="n">
-        <v>0.2556787286295783</v>
+        <v>0.2571463519840986</v>
       </c>
       <c r="K361" t="n">
-        <v>0.3732909437991843</v>
+        <v>0.3754336738967839</v>
       </c>
       <c r="L361" t="n">
-        <v>1.486381926512897</v>
+        <v>1.477693596254136</v>
       </c>
       <c r="M361" t="n">
-        <v>1.140327129687919</v>
+        <v>1.14687272984908</v>
       </c>
       <c r="N361" t="n">
         <v>0</v>
@@ -15757,25 +15757,25 @@
         </is>
       </c>
       <c r="G365" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="H365" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="I365" t="n">
-        <v>0.2857252170371667</v>
+        <v>0.2880917171917416</v>
       </c>
       <c r="J365" t="n">
-        <v>0.2971159660885698</v>
+        <v>0.2912943757083156</v>
       </c>
       <c r="K365" t="n">
-        <v>0.4171588168742634</v>
+        <v>0.4206139070999428</v>
       </c>
       <c r="L365" t="n">
-        <v>1.274334467985764</v>
+        <v>1.284889058675168</v>
       </c>
       <c r="M365" t="n">
-        <v>1.308506715139973</v>
+        <v>1.29449703422489</v>
       </c>
       <c r="N365" t="n">
         <v>3</v>
@@ -15849,25 +15849,25 @@
         </is>
       </c>
       <c r="G367" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="H367" t="n">
-        <v>91.11751334180001</v>
+        <v>90.496326364</v>
       </c>
       <c r="I367" t="n">
-        <v>0.2626345516117167</v>
+        <v>0.2773191524520125</v>
       </c>
       <c r="J367" t="n">
-        <v>0.3539190030351769</v>
+        <v>0.3177948849680494</v>
       </c>
       <c r="K367" t="n">
-        <v>0.3834464453531064</v>
+        <v>0.4048859625799382</v>
       </c>
       <c r="L367" t="n">
-        <v>1.171350100188256</v>
+        <v>1.236843419935976</v>
       </c>
       <c r="M367" t="n">
-        <v>1.445203454458637</v>
+        <v>1.358270617484086</v>
       </c>
       <c r="N367" t="n">
         <v>0</v>
@@ -15980,25 +15980,25 @@
         </is>
       </c>
       <c r="G370" t="n">
-        <v>85.65611116149999</v>
+        <v>85.21581244470001</v>
       </c>
       <c r="H370" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="I370" t="n">
-        <v>0.3423894451338487</v>
+        <v>0.3408047219652566</v>
       </c>
       <c r="J370" t="n">
-        <v>0.2673213637667282</v>
+        <v>0.267965560176725</v>
       </c>
       <c r="K370" t="n">
-        <v>0.3902891910994231</v>
+        <v>0.3912297178580185</v>
       </c>
       <c r="L370" t="n">
-        <v>1.417457526500969</v>
+        <v>1.413643883753788</v>
       </c>
       <c r="M370" t="n">
-        <v>1.192253282399607</v>
+        <v>1.195126398388193</v>
       </c>
       <c r="N370" t="n">
         <v>1</v>
@@ -16228,25 +16228,25 @@
         </is>
       </c>
       <c r="G376" t="n">
-        <v>87.3498746941</v>
+        <v>86.9412866479</v>
       </c>
       <c r="H376" t="n">
-        <v>85.6051744865</v>
+        <v>86.0987176703</v>
       </c>
       <c r="I376" t="n">
-        <v>0.4621285922372467</v>
+        <v>0.4297216256396926</v>
       </c>
       <c r="J376" t="n">
-        <v>0.2186469137246965</v>
+        <v>0.2318204773822388</v>
       </c>
       <c r="K376" t="n">
-        <v>0.3192244940380568</v>
+        <v>0.3384578969780686</v>
       </c>
       <c r="L376" t="n">
-        <v>1.705610270749797</v>
+        <v>1.627622773897146</v>
       </c>
       <c r="M376" t="n">
-        <v>0.9751652352121463</v>
+        <v>1.033919329124785</v>
       </c>
       <c r="N376" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
MAIN WORKS and I added laliga data and it all works!!!!!!!
</commit_message>
<xml_diff>
--- a/Sezon/PremierLeague2025_26.xlsx
+++ b/Sezon/PremierLeague2025_26.xlsx
@@ -1007,7 +1007,9 @@
       <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="n">
+        <v>9</v>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>Arsenal</t>
@@ -1018,9 +1020,17 @@
           <t>Crystal Palace</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
       <c r="G14" t="n">
         <v>100</v>
       </c>
@@ -1042,8 +1052,12 @@
       <c r="M14" t="n">
         <v>0.63052349285876</v>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>3</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1804,7 +1818,9 @@
       <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
+      <c r="A33" t="n">
+        <v>10</v>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>Burnley</t>
@@ -1815,9 +1831,17 @@
           <t>Arsenal</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
       <c r="G33" t="n">
         <v>85.21581244470001</v>
       </c>
@@ -1839,8 +1863,12 @@
       <c r="M33" t="n">
         <v>2.214731399226153</v>
       </c>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2183,7 +2211,9 @@
       <c r="O41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="n">
+        <v>10</v>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>Manchester City</t>
@@ -2194,9 +2224,17 @@
           <t>AFC Bournemouth</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
       <c r="G42" t="n">
         <v>97.5382271762</v>
       </c>
@@ -2218,8 +2256,12 @@
       <c r="M42" t="n">
         <v>0.6814232717844892</v>
       </c>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
+      <c r="N42" t="n">
+        <v>3</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -2810,7 +2852,9 @@
       <c r="O56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
+      <c r="A57" t="n">
+        <v>9</v>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>Aston Villa</t>
@@ -2821,9 +2865,17 @@
           <t>Manchester City</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
       <c r="G57" t="n">
         <v>93.2242913626</v>
       </c>
@@ -2845,8 +2897,12 @@
       <c r="M57" t="n">
         <v>1.331057943502569</v>
       </c>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
+      <c r="N57" t="n">
+        <v>3</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4209,7 +4265,9 @@
       <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr"/>
+      <c r="A90" t="n">
+        <v>10</v>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
           <t>Liverpool</t>
@@ -4220,9 +4278,17 @@
           <t>Aston Villa</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>2</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
       <c r="G90" t="n">
         <v>97.0684976167</v>
       </c>
@@ -4244,8 +4310,12 @@
       <c r="M90" t="n">
         <v>0.8144998949270565</v>
       </c>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
+      <c r="N90" t="n">
+        <v>3</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -4666,7 +4736,9 @@
       <c r="O100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr"/>
+      <c r="A101" t="n">
+        <v>9</v>
+      </c>
       <c r="B101" t="inlineStr">
         <is>
           <t>Brentford</t>
@@ -4677,9 +4749,17 @@
           <t>Liverpool</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr"/>
+      <c r="D101" t="n">
+        <v>3</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
       <c r="G101" t="n">
         <v>90.496326364</v>
       </c>
@@ -4701,8 +4781,12 @@
       <c r="M101" t="n">
         <v>1.514295703016295</v>
       </c>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
+      <c r="N101" t="n">
+        <v>3</v>
+      </c>
+      <c r="O101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr"/>
@@ -6129,7 +6213,9 @@
       <c r="O135" t="inlineStr"/>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr"/>
+      <c r="A136" t="n">
+        <v>9</v>
+      </c>
       <c r="B136" t="inlineStr">
         <is>
           <t>AFC Bournemouth</t>
@@ -6140,9 +6226,17 @@
           <t>Nottingham Forest</t>
         </is>
       </c>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr"/>
-      <c r="F136" t="inlineStr"/>
+      <c r="D136" t="n">
+        <v>2</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>AFC Bournemouth</t>
+        </is>
+      </c>
       <c r="G136" t="n">
         <v>91.5882912066</v>
       </c>
@@ -6164,8 +6258,12 @@
       <c r="M136" t="n">
         <v>0.7772805380325811</v>
       </c>
-      <c r="N136" t="inlineStr"/>
-      <c r="O136" t="inlineStr"/>
+      <c r="N136" t="n">
+        <v>3</v>
+      </c>
+      <c r="O136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr"/>
@@ -6416,7 +6514,9 @@
       <c r="O142" t="inlineStr"/>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr"/>
+      <c r="A143" t="n">
+        <v>10</v>
+      </c>
       <c r="B143" t="inlineStr">
         <is>
           <t>Tottenham Hotspur</t>
@@ -6427,9 +6527,17 @@
           <t>Chelsea</t>
         </is>
       </c>
-      <c r="D143" t="inlineStr"/>
-      <c r="E143" t="inlineStr"/>
-      <c r="F143" t="inlineStr"/>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="n">
+        <v>1</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
       <c r="G143" t="n">
         <v>91.34868924840001</v>
       </c>
@@ -6451,11 +6559,17 @@
       <c r="M143" t="n">
         <v>1.250616638692154</v>
       </c>
-      <c r="N143" t="inlineStr"/>
-      <c r="O143" t="inlineStr"/>
+      <c r="N143" t="n">
+        <v>0</v>
+      </c>
+      <c r="O143" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr"/>
+      <c r="A144" t="n">
+        <v>9</v>
+      </c>
       <c r="B144" t="inlineStr">
         <is>
           <t>Chelsea</t>
@@ -6466,9 +6580,17 @@
           <t>Sunderland</t>
         </is>
       </c>
-      <c r="D144" t="inlineStr"/>
-      <c r="E144" t="inlineStr"/>
-      <c r="F144" t="inlineStr"/>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
+      <c r="E144" t="n">
+        <v>2</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Sunderland</t>
+        </is>
+      </c>
       <c r="G144" t="n">
         <v>94.2958640271</v>
       </c>
@@ -6490,8 +6612,12 @@
       <c r="M144" t="n">
         <v>0.5410186428587073</v>
       </c>
-      <c r="N144" t="inlineStr"/>
-      <c r="O144" t="inlineStr"/>
+      <c r="N144" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr"/>
@@ -8102,7 +8228,9 @@
       <c r="O182" t="inlineStr"/>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr"/>
+      <c r="A183" t="n">
+        <v>9</v>
+      </c>
       <c r="B183" t="inlineStr">
         <is>
           <t>Everton</t>
@@ -8113,9 +8241,17 @@
           <t>Tottenham Hotspur</t>
         </is>
       </c>
-      <c r="D183" t="inlineStr"/>
-      <c r="E183" t="inlineStr"/>
-      <c r="F183" t="inlineStr"/>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>3</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Tottenham Hotspur</t>
+        </is>
+      </c>
       <c r="G183" t="n">
         <v>88.7111050262</v>
       </c>
@@ -8137,8 +8273,12 @@
       <c r="M183" t="n">
         <v>1.23924403499715</v>
       </c>
-      <c r="N183" t="inlineStr"/>
-      <c r="O183" t="inlineStr"/>
+      <c r="N183" t="n">
+        <v>0</v>
+      </c>
+      <c r="O183" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr"/>
@@ -9175,7 +9315,9 @@
       <c r="O207" t="inlineStr"/>
     </row>
     <row r="208">
-      <c r="A208" t="inlineStr"/>
+      <c r="A208" t="n">
+        <v>10</v>
+      </c>
       <c r="B208" t="inlineStr">
         <is>
           <t>Sunderland</t>
@@ -9186,9 +9328,17 @@
           <t>Everton</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr"/>
-      <c r="E208" t="inlineStr"/>
-      <c r="F208" t="inlineStr"/>
+      <c r="D208" t="n">
+        <v>1</v>
+      </c>
+      <c r="E208" t="n">
+        <v>1</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
       <c r="G208" t="n">
         <v>85.7823829526</v>
       </c>
@@ -9210,8 +9360,12 @@
       <c r="M208" t="n">
         <v>1.261870235142902</v>
       </c>
-      <c r="N208" t="inlineStr"/>
-      <c r="O208" t="inlineStr"/>
+      <c r="N208" t="n">
+        <v>1</v>
+      </c>
+      <c r="O208" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr"/>
@@ -10521,7 +10675,9 @@
       <c r="O239" t="inlineStr"/>
     </row>
     <row r="240">
-      <c r="A240" t="inlineStr"/>
+      <c r="A240" t="n">
+        <v>10</v>
+      </c>
       <c r="B240" t="inlineStr">
         <is>
           <t>Crystal Palace</t>
@@ -10532,9 +10688,17 @@
           <t>Brentford</t>
         </is>
       </c>
-      <c r="D240" t="inlineStr"/>
-      <c r="E240" t="inlineStr"/>
-      <c r="F240" t="inlineStr"/>
+      <c r="D240" t="n">
+        <v>2</v>
+      </c>
+      <c r="E240" t="n">
+        <v>0</v>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
       <c r="G240" t="n">
         <v>93.29711155859999</v>
       </c>
@@ -10556,8 +10720,12 @@
       <c r="M240" t="n">
         <v>0.8915131361579346</v>
       </c>
-      <c r="N240" t="inlineStr"/>
-      <c r="O240" t="inlineStr"/>
+      <c r="N240" t="n">
+        <v>3</v>
+      </c>
+      <c r="O240" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr"/>
@@ -10939,7 +11107,9 @@
       <c r="O249" t="inlineStr"/>
     </row>
     <row r="250">
-      <c r="A250" t="inlineStr"/>
+      <c r="A250" t="n">
+        <v>9</v>
+      </c>
       <c r="B250" t="inlineStr">
         <is>
           <t>Manchester United</t>
@@ -10950,9 +11120,17 @@
           <t>Brighton &amp; Hove Albion</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr"/>
-      <c r="E250" t="inlineStr"/>
-      <c r="F250" t="inlineStr"/>
+      <c r="D250" t="n">
+        <v>4</v>
+      </c>
+      <c r="E250" t="n">
+        <v>2</v>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Manchester United</t>
+        </is>
+      </c>
       <c r="G250" t="n">
         <v>90.8794818878</v>
       </c>
@@ -10974,8 +11152,12 @@
       <c r="M250" t="n">
         <v>1.149339330631851</v>
       </c>
-      <c r="N250" t="inlineStr"/>
-      <c r="O250" t="inlineStr"/>
+      <c r="N250" t="n">
+        <v>3</v>
+      </c>
+      <c r="O250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr"/>
@@ -11644,7 +11826,9 @@
       <c r="O266" t="inlineStr"/>
     </row>
     <row r="267">
-      <c r="A267" t="inlineStr"/>
+      <c r="A267" t="n">
+        <v>10</v>
+      </c>
       <c r="B267" t="inlineStr">
         <is>
           <t>Nottingham Forest</t>
@@ -11655,9 +11839,17 @@
           <t>Manchester United</t>
         </is>
       </c>
-      <c r="D267" t="inlineStr"/>
-      <c r="E267" t="inlineStr"/>
-      <c r="F267" t="inlineStr"/>
+      <c r="D267" t="n">
+        <v>2</v>
+      </c>
+      <c r="E267" t="n">
+        <v>2</v>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
       <c r="G267" t="n">
         <v>86.9412866479</v>
       </c>
@@ -11679,8 +11871,12 @@
       <c r="M267" t="n">
         <v>1.321997612120811</v>
       </c>
-      <c r="N267" t="inlineStr"/>
-      <c r="O267" t="inlineStr"/>
+      <c r="N267" t="n">
+        <v>1</v>
+      </c>
+      <c r="O267" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr"/>
@@ -12193,7 +12389,9 @@
       <c r="O279" t="inlineStr"/>
     </row>
     <row r="280">
-      <c r="A280" t="inlineStr"/>
+      <c r="A280" t="n">
+        <v>10</v>
+      </c>
       <c r="B280" t="inlineStr">
         <is>
           <t>Brighton &amp; Hove Albion</t>
@@ -12204,9 +12402,17 @@
           <t>Leeds United</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr"/>
-      <c r="E280" t="inlineStr"/>
-      <c r="F280" t="inlineStr"/>
+      <c r="D280" t="n">
+        <v>3</v>
+      </c>
+      <c r="E280" t="n">
+        <v>0</v>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Brighton &amp; Hove Albion</t>
+        </is>
+      </c>
       <c r="G280" t="n">
         <v>92.0576470387</v>
       </c>
@@ -12228,8 +12434,12 @@
       <c r="M280" t="n">
         <v>0.6393308553257451</v>
       </c>
-      <c r="N280" t="inlineStr"/>
-      <c r="O280" t="inlineStr"/>
+      <c r="N280" t="n">
+        <v>3</v>
+      </c>
+      <c r="O280" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr"/>
@@ -14113,7 +14323,9 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" t="inlineStr"/>
+      <c r="A326" t="n">
+        <v>9</v>
+      </c>
       <c r="B326" t="inlineStr">
         <is>
           <t>Newcastle United</t>
@@ -14124,9 +14336,17 @@
           <t>Fulham</t>
         </is>
       </c>
-      <c r="D326" t="inlineStr"/>
-      <c r="E326" t="inlineStr"/>
-      <c r="F326" t="inlineStr"/>
+      <c r="D326" t="n">
+        <v>2</v>
+      </c>
+      <c r="E326" t="n">
+        <v>1</v>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Newcastle United</t>
+        </is>
+      </c>
       <c r="G326" t="n">
         <v>93.4578390827</v>
       </c>
@@ -14148,8 +14368,12 @@
       <c r="M326" t="n">
         <v>0.7561127378259371</v>
       </c>
-      <c r="N326" t="inlineStr"/>
-      <c r="O326" t="inlineStr"/>
+      <c r="N326" t="n">
+        <v>3</v>
+      </c>
+      <c r="O326" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr"/>
@@ -14570,7 +14794,9 @@
       <c r="O336" t="inlineStr"/>
     </row>
     <row r="337">
-      <c r="A337" t="inlineStr"/>
+      <c r="A337" t="n">
+        <v>10</v>
+      </c>
       <c r="B337" t="inlineStr">
         <is>
           <t>West Ham United</t>
@@ -14581,9 +14807,17 @@
           <t>Newcastle United</t>
         </is>
       </c>
-      <c r="D337" t="inlineStr"/>
-      <c r="E337" t="inlineStr"/>
-      <c r="F337" t="inlineStr"/>
+      <c r="D337" t="n">
+        <v>3</v>
+      </c>
+      <c r="E337" t="n">
+        <v>1</v>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>West Ham United</t>
+        </is>
+      </c>
       <c r="G337" t="n">
         <v>86.0987176703</v>
       </c>
@@ -14605,8 +14839,12 @@
       <c r="M337" t="n">
         <v>1.593645720954024</v>
       </c>
-      <c r="N337" t="inlineStr"/>
-      <c r="O337" t="inlineStr"/>
+      <c r="N337" t="n">
+        <v>3</v>
+      </c>
+      <c r="O337" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
@@ -15119,7 +15357,9 @@
       <c r="O349" t="inlineStr"/>
     </row>
     <row r="350">
-      <c r="A350" t="inlineStr"/>
+      <c r="A350" t="n">
+        <v>10</v>
+      </c>
       <c r="B350" t="inlineStr">
         <is>
           <t>Fulham</t>
@@ -15130,9 +15370,17 @@
           <t>Wolverhampton Wanderers</t>
         </is>
       </c>
-      <c r="D350" t="inlineStr"/>
-      <c r="E350" t="inlineStr"/>
-      <c r="F350" t="inlineStr"/>
+      <c r="D350" t="n">
+        <v>3</v>
+      </c>
+      <c r="E350" t="n">
+        <v>0</v>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
       <c r="G350" t="n">
         <v>88.55071952030001</v>
       </c>
@@ -15154,8 +15402,12 @@
       <c r="M350" t="n">
         <v>0.8110558805877301</v>
       </c>
-      <c r="N350" t="inlineStr"/>
-      <c r="O350" t="inlineStr"/>
+      <c r="N350" t="n">
+        <v>3</v>
+      </c>
+      <c r="O350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr"/>
@@ -15445,7 +15697,9 @@
       <c r="O357" t="inlineStr"/>
     </row>
     <row r="358">
-      <c r="A358" t="inlineStr"/>
+      <c r="A358" t="n">
+        <v>9</v>
+      </c>
       <c r="B358" t="inlineStr">
         <is>
           <t>Leeds United</t>
@@ -15456,9 +15710,17 @@
           <t>West Ham United</t>
         </is>
       </c>
-      <c r="D358" t="inlineStr"/>
-      <c r="E358" t="inlineStr"/>
-      <c r="F358" t="inlineStr"/>
+      <c r="D358" t="n">
+        <v>2</v>
+      </c>
+      <c r="E358" t="n">
+        <v>1</v>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>Leeds United</t>
+        </is>
+      </c>
       <c r="G358" t="n">
         <v>85.1864986245</v>
       </c>
@@ -15480,8 +15742,12 @@
       <c r="M358" t="n">
         <v>1.147040080436756</v>
       </c>
-      <c r="N358" t="inlineStr"/>
-      <c r="O358" t="inlineStr"/>
+      <c r="N358" t="n">
+        <v>3</v>
+      </c>
+      <c r="O358" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr"/>
@@ -16164,7 +16430,9 @@
       <c r="O374" t="inlineStr"/>
     </row>
     <row r="375">
-      <c r="A375" t="inlineStr"/>
+      <c r="A375" t="n">
+        <v>9</v>
+      </c>
       <c r="B375" t="inlineStr">
         <is>
           <t>Wolverhampton Wanderers</t>
@@ -16175,9 +16443,17 @@
           <t>Burnley</t>
         </is>
       </c>
-      <c r="D375" t="inlineStr"/>
-      <c r="E375" t="inlineStr"/>
-      <c r="F375" t="inlineStr"/>
+      <c r="D375" t="n">
+        <v>2</v>
+      </c>
+      <c r="E375" t="n">
+        <v>3</v>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
       <c r="G375" t="n">
         <v>84.31203815969999</v>
       </c>
@@ -16199,8 +16475,12 @@
       <c r="M375" t="n">
         <v>1.14863637284857</v>
       </c>
-      <c r="N375" t="inlineStr"/>
-      <c r="O375" t="inlineStr"/>
+      <c r="N375" t="n">
+        <v>0</v>
+      </c>
+      <c r="O375" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="n">

</xml_diff>